<commit_message>
Atualizado em 18/02/2021 - 22h44
</commit_message>
<xml_diff>
--- a/UFxREG.xlsx
+++ b/UFxREG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juliano\Google Drive\Mestrado em Engenharia de Produção e Manufatura - Unicamp\PO450 - Introdução ao Aprendizado de Máquina e Mineração de Dados\000. Pré-disciplina\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6995A0D7-C504-4910-8F74-B8AD78EB884F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55514B07-A8FB-4D4B-8541-46F4DFBF659A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{873A64FF-F424-40F4-9811-954572315E4D}"/>
   </bookViews>
@@ -39,15 +39,9 @@
     <t>Rondônia</t>
   </si>
   <si>
-    <t>RO </t>
-  </si>
-  <si>
     <t>Acre </t>
   </si>
   <si>
-    <t>AC </t>
-  </si>
-  <si>
     <t>Amazonas</t>
   </si>
   <si>
@@ -57,27 +51,15 @@
     <t>Roraima </t>
   </si>
   <si>
-    <t>RR </t>
-  </si>
-  <si>
     <t>Pará </t>
   </si>
   <si>
-    <t>PA </t>
-  </si>
-  <si>
     <t>Amapá </t>
   </si>
   <si>
-    <t>AP </t>
-  </si>
-  <si>
     <t>Tocantins </t>
   </si>
   <si>
-    <t>TO </t>
-  </si>
-  <si>
     <t>Maranhão </t>
   </si>
   <si>
@@ -99,27 +81,15 @@
     <t>Rio Grande do Norte </t>
   </si>
   <si>
-    <t>RN </t>
-  </si>
-  <si>
     <t>Paraíba </t>
   </si>
   <si>
-    <t>PB </t>
-  </si>
-  <si>
     <t>Pernambuco </t>
   </si>
   <si>
-    <t>PE </t>
-  </si>
-  <si>
     <t>Alagoas </t>
   </si>
   <si>
-    <t>AL </t>
-  </si>
-  <si>
     <t>Sergipe</t>
   </si>
   <si>
@@ -220,6 +190,36 @@
   </si>
   <si>
     <t>REG</t>
+  </si>
+  <si>
+    <t>RO</t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>RR</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>AP</t>
+  </si>
+  <si>
+    <t>TO</t>
+  </si>
+  <si>
+    <t>RN</t>
+  </si>
+  <si>
+    <t>PB</t>
+  </si>
+  <si>
+    <t>PE</t>
+  </si>
+  <si>
+    <t>AL</t>
   </si>
 </sst>
 </file>
@@ -577,30 +577,30 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -611,10 +611,10 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -622,13 +622,13 @@
         <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>3</v>
+        <v>53</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -636,13 +636,13 @@
         <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -650,13 +650,13 @@
         <v>14</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -664,13 +664,13 @@
         <v>15</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>9</v>
+        <v>55</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -678,13 +678,13 @@
         <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>11</v>
+        <v>56</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -692,13 +692,13 @@
         <v>17</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -706,13 +706,13 @@
         <v>21</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -720,13 +720,13 @@
         <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -734,13 +734,13 @@
         <v>23</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -748,13 +748,13 @@
         <v>24</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -762,13 +762,13 @@
         <v>25</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -776,13 +776,13 @@
         <v>26</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -790,13 +790,13 @@
         <v>27</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -804,13 +804,13 @@
         <v>28</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -818,13 +818,13 @@
         <v>29</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -832,13 +832,13 @@
         <v>31</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -846,13 +846,13 @@
         <v>32</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -860,13 +860,13 @@
         <v>33</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -874,13 +874,13 @@
         <v>35</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -888,13 +888,13 @@
         <v>41</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -902,13 +902,13 @@
         <v>42</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -916,13 +916,13 @@
         <v>43</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -930,13 +930,13 @@
         <v>50</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -944,13 +944,13 @@
         <v>51</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -958,13 +958,13 @@
         <v>52</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -972,13 +972,13 @@
         <v>53</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>